<commit_message>
updated list and plots for new 2SK82 parts
</commit_message>
<xml_diff>
--- a/Sony_2SJ28_2SK82_list.xlsx
+++ b/Sony_2SJ28_2SK82_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t xml:space="preserve">Sony 2SJ28 and 2SK82 VFET List</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">2SJ28_2</t>
   </si>
   <si>
-    <t xml:space="preserve">available</t>
+    <t xml:space="preserve">on hold</t>
   </si>
   <si>
     <t xml:space="preserve">2SJ28_3</t>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t xml:space="preserve">2SK82_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2SK82_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2SK82_27</t>
   </si>
 </sst>
 </file>
@@ -343,10 +349,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ42"/>
+  <dimension ref="A1:AMJ53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G32" activeCellId="0" sqref="G32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,7 +813,7 @@
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="18" t="n">
+      <c r="B37" s="2" t="n">
         <v>-4.816</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -818,7 +824,7 @@
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="18" t="n">
+      <c r="B38" s="2" t="n">
         <v>-6.745</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -829,7 +835,7 @@
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="18" t="n">
+      <c r="B39" s="2" t="n">
         <v>-7.004</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -840,7 +846,7 @@
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="18" t="n">
+      <c r="B40" s="2" t="n">
         <v>-7.481</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -851,7 +857,7 @@
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="18" t="n">
+      <c r="B41" s="2" t="n">
         <v>-7.474</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -862,12 +868,62 @@
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="18" t="n">
+      <c r="B42" s="2" t="n">
         <v>-5.845</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="18" t="n">
+        <v>-6.425</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="18" t="n">
+        <v>-4.336</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0"/>
+      <c r="B52" s="0"/>
+      <c r="C52" s="0"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0"/>
+      <c r="B53" s="0"/>
+      <c r="C53" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>